<commit_message>
review notebook and clean
</commit_message>
<xml_diff>
--- a/results/financial_model.xlsx
+++ b/results/financial_model.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\Documents\GitHub\time_series_padova\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CE69DD4-FBEE-4667-98B3-0F227A9B6128}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F91F9AE-D3A8-4E06-9D82-6181365AEED7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="forecast" sheetId="1" r:id="rId1"/>
@@ -337,13 +337,13 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="8">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="0.0%"/>
-    <numFmt numFmtId="167" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="168" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;?_);@_)"/>
-    <numFmt numFmtId="169" formatCode="dd/mm/yy"/>
-    <numFmt numFmtId="172" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="173" formatCode="0.000%"/>
-    <numFmt numFmtId="175" formatCode="0.00\x"/>
+    <numFmt numFmtId="164" formatCode="0.0%"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;?_);@_)"/>
+    <numFmt numFmtId="167" formatCode="dd/mm/yy"/>
+    <numFmt numFmtId="168" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="169" formatCode="0.000%"/>
+    <numFmt numFmtId="170" formatCode="0.00\x"/>
   </numFmts>
   <fonts count="35" x14ac:knownFonts="1">
     <font>
@@ -585,7 +585,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -613,6 +613,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF002060"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -743,7 +749,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -779,33 +785,32 @@
     <xf numFmtId="10" fontId="10" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="3" fontId="13" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="3" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="3" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="10" fontId="14" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="167" fontId="16" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="167" fontId="16" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="16" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="16" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="167" fontId="16" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="16" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="17" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="15" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="167" fontId="16" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="167" fontId="17" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="16" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="17" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="15" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="16" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="17" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="16" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="3" fontId="18" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="167" fontId="19" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="19" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="167" fontId="20" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="167" fontId="21" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="22" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="169" fontId="24" fillId="4" borderId="4" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="20" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="21" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="22" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="24" fillId="4" borderId="4" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="25" fillId="2" borderId="0" xfId="3" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="25" fillId="2" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -817,23 +822,20 @@
     <xf numFmtId="0" fontId="29" fillId="2" borderId="0" xfId="3" applyFont="1" applyFill="1"/>
     <xf numFmtId="3" fontId="29" fillId="2" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="28" fillId="2" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="2" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="28" fillId="2" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="30" fillId="2" borderId="4" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="28" fillId="2" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="172" fontId="28" fillId="2" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="173" fontId="28" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="28" fillId="2" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="168" fontId="28" fillId="2" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="169" fontId="28" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="31" fillId="2" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="43" fontId="31" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="31" fillId="2" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="31" fillId="2" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="31" fillId="2" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="3" fontId="32" fillId="2" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="3" fontId="33" fillId="2" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -847,26 +849,26 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="2" borderId="8" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="29" fillId="2" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="29" fillId="2" borderId="9" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="28" fillId="2" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="29" fillId="2" borderId="8" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="175" fontId="10" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="175" fontId="0" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="170" fontId="10" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="170" fontId="0" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="3" fontId="7" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="8" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="8" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="8" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="34" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="26" fillId="2" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="10" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
@@ -2061,7 +2063,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:D39"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2:B39"/>
     </sheetView>
   </sheetViews>
@@ -2352,8 +2354,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{314C7F96-EC5F-4760-9CB2-5CA48DBFFB51}">
   <dimension ref="B1:F75"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B75"/>
+    <sheetView topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="F63" sqref="F63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3706,8 +3708,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1B44F11-AD96-4F90-96F3-54D69B79CC8C}">
   <dimension ref="B1:K42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3721,36 +3723,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:10" ht="18" x14ac:dyDescent="0.35">
-      <c r="B1" s="86" t="s">
+      <c r="B1" s="80" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B4" s="49" t="s">
+      <c r="B4" s="48" t="s">
         <v>47</v>
       </c>
-      <c r="C4" s="49" t="s">
+      <c r="C4" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="49" t="s">
+      <c r="D4" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="49" t="s">
+      <c r="E4" s="48" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="49" t="s">
+      <c r="F4" s="48" t="s">
         <v>19</v>
       </c>
-      <c r="G4" s="49" t="s">
+      <c r="G4" s="48" t="s">
         <v>20</v>
       </c>
-      <c r="H4" s="49" t="s">
+      <c r="H4" s="48" t="s">
         <v>21</v>
       </c>
-      <c r="I4" s="49" t="s">
+      <c r="I4" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="J4" s="49" t="s">
+      <c r="J4" s="48" t="s">
         <v>23</v>
       </c>
     </row>
@@ -3799,27 +3801,27 @@
       <c r="D6" s="11">
         <v>549003232</v>
       </c>
-      <c r="E6" s="21">
+      <c r="E6" s="10">
         <f>+E$5*E20</f>
         <v>576662948.24550498</v>
       </c>
-      <c r="F6" s="21">
+      <c r="F6" s="10">
         <f t="shared" ref="F6:J6" si="0">+F$5*F20</f>
         <v>622897867.89999998</v>
       </c>
-      <c r="G6" s="21">
+      <c r="G6" s="10">
         <f t="shared" si="0"/>
         <v>690876603.24639404</v>
       </c>
-      <c r="H6" s="21">
+      <c r="H6" s="10">
         <f t="shared" si="0"/>
         <v>761805505.78431547</v>
       </c>
-      <c r="I6" s="21">
+      <c r="I6" s="10">
         <f t="shared" si="0"/>
         <v>840016329.85727501</v>
       </c>
-      <c r="J6" s="21">
+      <c r="J6" s="10">
         <f t="shared" si="0"/>
         <v>926256674.53060591</v>
       </c>
@@ -3834,27 +3836,27 @@
       <c r="D7" s="11">
         <v>162898264</v>
       </c>
-      <c r="E7" s="21">
+      <c r="E7" s="10">
         <f t="shared" ref="E7:J7" si="1">+E$5*E21</f>
         <v>116344322.90013431</v>
       </c>
-      <c r="F7" s="21">
+      <c r="F7" s="10">
         <f t="shared" si="1"/>
         <v>173858236.74531502</v>
       </c>
-      <c r="G7" s="21">
+      <c r="G7" s="10">
         <f t="shared" si="1"/>
         <v>173816091.82948503</v>
       </c>
-      <c r="H7" s="21">
+      <c r="H7" s="10">
         <f t="shared" si="1"/>
         <v>202144976.51145732</v>
       </c>
-      <c r="I7" s="21">
+      <c r="I7" s="10">
         <f t="shared" si="1"/>
         <v>217118013.6887739</v>
       </c>
-      <c r="J7" s="21">
+      <c r="J7" s="10">
         <f t="shared" si="1"/>
         <v>242595260.80792299</v>
       </c>
@@ -3869,27 +3871,27 @@
       <c r="D8" s="11">
         <v>696655420</v>
       </c>
-      <c r="E8" s="21">
+      <c r="E8" s="10">
         <f t="shared" ref="E8:J8" si="2">+E$5*E22</f>
         <v>754336156.44720101</v>
       </c>
-      <c r="F8" s="21">
+      <c r="F8" s="10">
         <f t="shared" si="2"/>
         <v>800868687.30000007</v>
       </c>
-      <c r="G8" s="21">
+      <c r="G8" s="10">
         <f t="shared" si="2"/>
         <v>888269918.45964956</v>
       </c>
-      <c r="H8" s="21">
+      <c r="H8" s="10">
         <f t="shared" si="2"/>
         <v>979464221.72269142</v>
       </c>
-      <c r="I8" s="21">
+      <c r="I8" s="10">
         <f t="shared" si="2"/>
         <v>1080020995.5307822</v>
       </c>
-      <c r="J8" s="21">
+      <c r="J8" s="10">
         <f t="shared" si="2"/>
         <v>1190901438.6822076</v>
       </c>
@@ -3904,33 +3906,33 @@
       <c r="D9" s="11">
         <v>10478117</v>
       </c>
-      <c r="E9" s="21">
+      <c r="E9" s="10">
         <f t="shared" ref="E9:J9" si="3">+E$5*E23</f>
         <v>8485468.5683122464</v>
       </c>
-      <c r="F9" s="21">
+      <c r="F9" s="10">
         <f>+F$5*F23</f>
         <v>11784011.128590522</v>
       </c>
-      <c r="G9" s="21">
+      <c r="G9" s="10">
         <f t="shared" si="3"/>
         <v>12180127.253233457</v>
       </c>
-      <c r="H9" s="21">
+      <c r="H9" s="10">
         <f t="shared" si="3"/>
         <v>13921236.677034864</v>
       </c>
-      <c r="I9" s="21">
+      <c r="I9" s="10">
         <f t="shared" si="3"/>
         <v>15079958.159269309</v>
       </c>
-      <c r="J9" s="21">
+      <c r="J9" s="10">
         <f t="shared" si="3"/>
         <v>16777280.620239891</v>
       </c>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B10" s="22" t="s">
+      <c r="B10" s="21" t="s">
         <v>13</v>
       </c>
       <c r="C10" s="19">
@@ -3974,27 +3976,27 @@
       <c r="D11" s="11">
         <v>77984134</v>
       </c>
-      <c r="E11" s="21">
+      <c r="E11" s="10">
         <f t="shared" ref="E11:J11" si="5">+E$5*E25</f>
         <v>67341799.500942007</v>
       </c>
-      <c r="F11" s="21">
+      <c r="F11" s="10">
         <f t="shared" si="5"/>
         <v>90215400.058535814</v>
       </c>
-      <c r="G11" s="21">
+      <c r="G11" s="10">
         <f t="shared" si="5"/>
         <v>94830772.885556638</v>
       </c>
-      <c r="H11" s="21">
+      <c r="H11" s="10">
         <f t="shared" si="5"/>
         <v>107450110.42400318</v>
       </c>
-      <c r="I11" s="21">
+      <c r="I11" s="10">
         <f t="shared" si="5"/>
         <v>116891701.61215426</v>
       </c>
-      <c r="J11" s="21">
+      <c r="J11" s="10">
         <f t="shared" si="5"/>
         <v>129768896.80965064</v>
       </c>
@@ -4070,7 +4072,7 @@
       </c>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B14" s="22" t="s">
+      <c r="B14" s="21" t="s">
         <v>17</v>
       </c>
       <c r="C14" s="19">
@@ -4141,35 +4143,35 @@
       <c r="B17" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="C17" s="21">
+      <c r="C17" s="10">
         <f>+C5/CF!$C$38</f>
         <v>209101.9859090909</v>
       </c>
-      <c r="D17" s="21">
+      <c r="D17" s="10">
         <f>+D5/CF!$C$38</f>
         <v>316548.9197727273</v>
       </c>
-      <c r="E17" s="21">
+      <c r="E17" s="10">
         <f>+E5/CF!$C$38</f>
         <v>337173.35546247731</v>
       </c>
-      <c r="F17" s="21">
+      <c r="F17" s="10">
         <f>+F5/CF!$C$38</f>
         <v>404479.13500000001</v>
       </c>
-      <c r="G17" s="21">
+      <c r="G17" s="10">
         <f>+G5/CF!$C$38</f>
         <v>448621.17093921691</v>
       </c>
-      <c r="H17" s="21">
+      <c r="H17" s="10">
         <f>+H5/CF!$C$38</f>
         <v>494678.89985994512</v>
       </c>
-      <c r="I17" s="21">
+      <c r="I17" s="10">
         <f>+I5/CF!$C$38</f>
         <v>545465.14925797086</v>
       </c>
-      <c r="J17" s="21">
+      <c r="J17" s="10">
         <f>+J5/CF!$C$38</f>
         <v>601465.37307182199</v>
       </c>
@@ -4195,7 +4197,7 @@
         <f>+AVERAGE(C20:D20)</f>
         <v>0.38870141676859937</v>
       </c>
-      <c r="F20" s="18">
+      <c r="F20" s="82">
         <v>0.35</v>
       </c>
       <c r="G20" s="16">
@@ -4268,7 +4270,7 @@
         <f>+AVERAGE(C22:D22)</f>
         <v>0.50846258394596344</v>
       </c>
-      <c r="F22" s="18">
+      <c r="F22" s="82">
         <v>0.45</v>
       </c>
       <c r="G22" s="16">
@@ -4443,10 +4445,10 @@
       <c r="B31" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="C31" s="34">
+      <c r="C31" s="33">
         <v>1556658</v>
       </c>
-      <c r="D31" s="34">
+      <c r="D31" s="33">
         <v>1556658</v>
       </c>
       <c r="E31" s="10">
@@ -4514,7 +4516,7 @@
       <c r="K32" s="10"/>
     </row>
     <row r="33" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B33" s="22" t="s">
+      <c r="B33" s="21" t="s">
         <v>36</v>
       </c>
       <c r="C33" s="20">
@@ -4598,7 +4600,7 @@
         <v>37</v>
       </c>
       <c r="C37" s="14">
-        <f t="shared" ref="C37:D37" si="24">+C32/C$5</f>
+        <f t="shared" ref="C37" si="24">+C32/C$5</f>
         <v>3.4793596988771699E-2</v>
       </c>
       <c r="D37" s="14">
@@ -4720,7 +4722,7 @@
       </c>
     </row>
     <row r="42" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B42" s="22" t="s">
+      <c r="B42" s="21" t="s">
         <v>40</v>
       </c>
       <c r="C42" s="20">
@@ -4780,7 +4782,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:10" ht="18" x14ac:dyDescent="0.35">
-      <c r="B1" s="86" t="s">
+      <c r="B1" s="80" t="s">
         <v>31</v>
       </c>
     </row>
@@ -4788,31 +4790,31 @@
       <c r="D3" s="12"/>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B4" s="49" t="s">
+      <c r="B4" s="48" t="s">
         <v>47</v>
       </c>
-      <c r="C4" s="49" t="s">
+      <c r="C4" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="49" t="s">
+      <c r="D4" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="49" t="s">
+      <c r="E4" s="48" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="49" t="s">
+      <c r="F4" s="48" t="s">
         <v>19</v>
       </c>
-      <c r="G4" s="49" t="s">
+      <c r="G4" s="48" t="s">
         <v>20</v>
       </c>
-      <c r="H4" s="49" t="s">
+      <c r="H4" s="48" t="s">
         <v>21</v>
       </c>
-      <c r="I4" s="49" t="s">
+      <c r="I4" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="J4" s="49" t="s">
+      <c r="J4" s="48" t="s">
         <v>23</v>
       </c>
     </row>
@@ -4826,27 +4828,27 @@
       <c r="D5" s="11">
         <v>111867928</v>
       </c>
-      <c r="E5" s="21">
+      <c r="E5" s="10">
         <f>+D5*(1+E$14)</f>
         <v>119156573.58576947</v>
       </c>
-      <c r="F5" s="21">
+      <c r="F5" s="10">
         <f t="shared" ref="F5:J5" si="0">+E5*(1+F$14)</f>
         <v>142942338.21479845</v>
       </c>
-      <c r="G5" s="21">
+      <c r="G5" s="10">
         <f t="shared" si="0"/>
         <v>158542069.53521216</v>
       </c>
-      <c r="H5" s="21">
+      <c r="H5" s="10">
         <f t="shared" si="0"/>
         <v>174818803.96996176</v>
       </c>
-      <c r="I5" s="21">
+      <c r="I5" s="10">
         <f t="shared" si="0"/>
         <v>192766590.66633534</v>
       </c>
-      <c r="J5" s="21">
+      <c r="J5" s="10">
         <f t="shared" si="0"/>
         <v>212556988.34038082</v>
       </c>
@@ -4861,33 +4863,33 @@
       <c r="D6" s="11">
         <v>90576197</v>
       </c>
-      <c r="E6" s="21">
+      <c r="E6" s="10">
         <f t="shared" ref="E6:J6" si="1">+D6*(1+E$14)</f>
         <v>96477600.648415089</v>
       </c>
-      <c r="F6" s="21">
+      <c r="F6" s="10">
         <f t="shared" si="1"/>
         <v>115736240.20089307</v>
       </c>
-      <c r="G6" s="21">
+      <c r="G6" s="10">
         <f t="shared" si="1"/>
         <v>128366887.45150506</v>
       </c>
-      <c r="H6" s="21">
+      <c r="H6" s="10">
         <f t="shared" si="1"/>
         <v>141545684.36887142</v>
       </c>
-      <c r="I6" s="21">
+      <c r="I6" s="10">
         <f t="shared" si="1"/>
         <v>156077483.54123753</v>
       </c>
-      <c r="J6" s="21">
+      <c r="J6" s="10">
         <f t="shared" si="1"/>
         <v>172101191.05491102</v>
       </c>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B7" s="22" t="s">
+      <c r="B7" s="21" t="s">
         <v>26</v>
       </c>
       <c r="C7" s="19">
@@ -4931,27 +4933,27 @@
       <c r="D8" s="11">
         <v>185001855</v>
       </c>
-      <c r="E8" s="21">
+      <c r="E8" s="10">
         <f t="shared" ref="E8:J8" si="3">+D8*(1+E$14)</f>
         <v>197055470.16845933</v>
       </c>
-      <c r="F8" s="21">
+      <c r="F8" s="10">
         <f t="shared" si="3"/>
         <v>236391235.63435537</v>
       </c>
-      <c r="G8" s="21">
+      <c r="G8" s="10">
         <f t="shared" si="3"/>
         <v>262189328.82669672</v>
       </c>
-      <c r="H8" s="21">
+      <c r="H8" s="10">
         <f t="shared" si="3"/>
         <v>289107017.5477308</v>
       </c>
-      <c r="I8" s="21">
+      <c r="I8" s="10">
         <f t="shared" si="3"/>
         <v>318788212.96571898</v>
       </c>
-      <c r="J8" s="21">
+      <c r="J8" s="10">
         <f t="shared" si="3"/>
         <v>351516630.71996665</v>
       </c>
@@ -4966,33 +4968,33 @@
       <c r="D9" s="11">
         <v>5038459</v>
       </c>
-      <c r="E9" s="21">
+      <c r="E9" s="10">
         <f t="shared" ref="E9:J9" si="4">+D9*(1+E$14)</f>
         <v>5366734.875007093</v>
       </c>
-      <c r="F9" s="21">
+      <c r="F9" s="10">
         <f t="shared" si="4"/>
         <v>6438030.3035504073</v>
       </c>
-      <c r="G9" s="21">
+      <c r="G9" s="10">
         <f t="shared" si="4"/>
         <v>7140632.095450229</v>
       </c>
-      <c r="H9" s="21">
+      <c r="H9" s="10">
         <f t="shared" si="4"/>
         <v>7873725.6690021949</v>
       </c>
-      <c r="I9" s="21">
+      <c r="I9" s="10">
         <f t="shared" si="4"/>
         <v>8682082.3537744712</v>
       </c>
-      <c r="J9" s="21">
+      <c r="J9" s="10">
         <f t="shared" si="4"/>
         <v>9573429.0431882013</v>
       </c>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B10" s="22" t="s">
+      <c r="B10" s="21" t="s">
         <v>29</v>
       </c>
       <c r="C10" s="19">
@@ -5070,27 +5072,27 @@
       <c r="B14" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="E14" s="23">
+      <c r="E14" s="22">
         <f>+IS!E15</f>
         <v>6.5154023285114215E-2</v>
       </c>
-      <c r="F14" s="23">
+      <c r="F14" s="22">
         <f>+IS!F15</f>
         <v>0.19961772912098596</v>
       </c>
-      <c r="G14" s="23">
+      <c r="G14" s="22">
         <f>+IS!G15</f>
         <v>0.10913303584674883</v>
       </c>
-      <c r="H14" s="23">
+      <c r="H14" s="22">
         <f>+IS!H15</f>
         <v>0.10266508115143869</v>
       </c>
-      <c r="I14" s="23">
+      <c r="I14" s="22">
         <f>+IS!I15</f>
         <v>0.10266508115143869</v>
       </c>
-      <c r="J14" s="23">
+      <c r="J14" s="22">
         <f>+IS!J15</f>
         <v>0.10266508115143869</v>
       </c>
@@ -5101,7 +5103,7 @@
       </c>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B16" s="22" t="s">
+      <c r="B16" s="21" t="s">
         <v>26</v>
       </c>
     </row>
@@ -5135,7 +5137,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68B502B8-38B1-4B53-AFCB-AAA416599912}">
   <dimension ref="B1:L52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+    <sheetView topLeftCell="A21" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -5153,420 +5155,420 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="18" x14ac:dyDescent="0.35">
-      <c r="B1" s="86" t="s">
+      <c r="B1" s="80" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B4" s="42" t="s">
+      <c r="B4" s="41" t="s">
         <v>43</v>
       </c>
-      <c r="C4" s="42"/>
-      <c r="D4" s="42"/>
-      <c r="E4" s="42"/>
-      <c r="F4" s="42"/>
-      <c r="G4" s="42"/>
-      <c r="H4" s="42"/>
-      <c r="I4" s="42"/>
-      <c r="J4" s="42"/>
-      <c r="K4" s="42"/>
+      <c r="C4" s="41"/>
+      <c r="D4" s="41"/>
+      <c r="E4" s="41"/>
+      <c r="F4" s="41"/>
+      <c r="G4" s="41"/>
+      <c r="H4" s="41"/>
+      <c r="I4" s="41"/>
+      <c r="J4" s="41"/>
+      <c r="K4" s="41"/>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B5" s="42" t="s">
+      <c r="B5" s="41" t="s">
         <v>62</v>
       </c>
-      <c r="C5" s="42"/>
-      <c r="D5" s="56">
+      <c r="C5" s="41"/>
+      <c r="D5" s="54">
         <v>0.35</v>
       </c>
-      <c r="E5" s="44"/>
-      <c r="F5" s="42" t="s">
+      <c r="E5" s="43"/>
+      <c r="F5" s="41" t="s">
         <v>63</v>
       </c>
-      <c r="G5" s="42"/>
-      <c r="H5" s="59">
+      <c r="G5" s="41"/>
+      <c r="H5" s="57">
         <v>6.8699999999999997E-2</v>
       </c>
-      <c r="I5" s="50" t="s">
+      <c r="I5" s="81" t="s">
         <v>64</v>
       </c>
-      <c r="J5" s="50"/>
-      <c r="K5" s="59">
+      <c r="J5" s="81"/>
+      <c r="K5" s="57">
         <v>0.03</v>
       </c>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B6" s="42" t="s">
+      <c r="B6" s="41" t="s">
         <v>65</v>
       </c>
-      <c r="C6" s="42"/>
-      <c r="D6" s="57">
+      <c r="C6" s="41"/>
+      <c r="D6" s="55">
         <v>1</v>
       </c>
-      <c r="E6" s="44"/>
-      <c r="F6" s="42" t="s">
+      <c r="E6" s="43"/>
+      <c r="F6" s="41" t="s">
         <v>66</v>
       </c>
-      <c r="G6" s="42"/>
-      <c r="H6" s="59">
+      <c r="G6" s="41"/>
+      <c r="H6" s="57">
         <v>4.7899999999999998E-2</v>
       </c>
-      <c r="I6" s="50" t="s">
+      <c r="I6" s="81" t="s">
         <v>67</v>
       </c>
-      <c r="J6" s="50"/>
-      <c r="K6" s="59">
+      <c r="J6" s="81"/>
+      <c r="K6" s="57">
         <v>0.08</v>
       </c>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B7" s="42" t="s">
+      <c r="B7" s="41" t="s">
         <v>68</v>
       </c>
-      <c r="C7" s="42"/>
-      <c r="D7" s="57">
+      <c r="C7" s="41"/>
+      <c r="D7" s="55">
         <v>0</v>
       </c>
-      <c r="E7" s="44"/>
-      <c r="F7" s="42" t="s">
+      <c r="E7" s="43"/>
+      <c r="F7" s="41" t="s">
         <v>69</v>
       </c>
-      <c r="G7" s="42"/>
-      <c r="H7" s="59">
+      <c r="G7" s="41"/>
+      <c r="H7" s="57">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="I7" s="44"/>
-      <c r="J7" s="42"/>
-      <c r="K7" s="42"/>
+      <c r="I7" s="43"/>
+      <c r="J7" s="41"/>
+      <c r="K7" s="41"/>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B8" s="42" t="s">
+      <c r="B8" s="41" t="s">
         <v>70</v>
       </c>
-      <c r="C8" s="42"/>
-      <c r="D8" s="58" t="s">
+      <c r="C8" s="41"/>
+      <c r="D8" s="56" t="s">
         <v>85</v>
       </c>
-      <c r="E8" s="44"/>
-      <c r="F8" s="42" t="s">
+      <c r="E8" s="43"/>
+      <c r="F8" s="41" t="s">
         <v>71</v>
       </c>
-      <c r="G8" s="42"/>
-      <c r="H8" s="59">
+      <c r="G8" s="41"/>
+      <c r="H8" s="57">
         <v>1.89E-2</v>
       </c>
-      <c r="I8" s="44"/>
-      <c r="J8" s="42"/>
-      <c r="K8" s="42"/>
+      <c r="I8" s="43"/>
+      <c r="J8" s="41"/>
+      <c r="K8" s="41"/>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B9" s="44"/>
-      <c r="C9" s="44"/>
-      <c r="D9" s="44"/>
-      <c r="E9" s="44"/>
-      <c r="F9" s="44"/>
-      <c r="G9" s="44"/>
-      <c r="H9" s="44"/>
-      <c r="I9" s="44"/>
-      <c r="J9" s="44"/>
-      <c r="K9" s="44"/>
+      <c r="B9" s="43"/>
+      <c r="C9" s="43"/>
+      <c r="D9" s="43"/>
+      <c r="E9" s="43"/>
+      <c r="F9" s="43"/>
+      <c r="G9" s="43"/>
+      <c r="H9" s="43"/>
+      <c r="I9" s="43"/>
+      <c r="J9" s="43"/>
+      <c r="K9" s="43"/>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B10" s="44"/>
-      <c r="C10" s="44"/>
-      <c r="D10" s="44"/>
-      <c r="E10" s="44"/>
-      <c r="F10" s="44"/>
-      <c r="G10" s="44"/>
-      <c r="H10" s="44"/>
-      <c r="I10" s="44"/>
-      <c r="J10" s="44"/>
-      <c r="K10" s="44"/>
+      <c r="B10" s="43"/>
+      <c r="C10" s="43"/>
+      <c r="D10" s="43"/>
+      <c r="E10" s="43"/>
+      <c r="F10" s="43"/>
+      <c r="G10" s="43"/>
+      <c r="H10" s="43"/>
+      <c r="I10" s="43"/>
+      <c r="J10" s="43"/>
+      <c r="K10" s="43"/>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B11" s="44"/>
-      <c r="C11" s="44"/>
-      <c r="D11" s="44"/>
-      <c r="E11" s="51"/>
-      <c r="F11" s="44"/>
-      <c r="G11" s="44"/>
-      <c r="H11" s="44"/>
-      <c r="I11" s="44"/>
-      <c r="J11" s="44"/>
-      <c r="K11" s="44"/>
+      <c r="B11" s="43"/>
+      <c r="C11" s="43"/>
+      <c r="D11" s="43"/>
+      <c r="E11" s="49"/>
+      <c r="F11" s="43"/>
+      <c r="G11" s="43"/>
+      <c r="H11" s="43"/>
+      <c r="I11" s="43"/>
+      <c r="J11" s="43"/>
+      <c r="K11" s="43"/>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B12" s="52" t="s">
+      <c r="B12" s="50" t="s">
         <v>72</v>
       </c>
-      <c r="C12" s="52" t="s">
+      <c r="C12" s="50" t="s">
         <v>73</v>
       </c>
-      <c r="D12" s="52" t="s">
+      <c r="D12" s="50" t="s">
         <v>74</v>
       </c>
-      <c r="E12" s="52"/>
-      <c r="F12" s="44"/>
-      <c r="G12" s="44"/>
-      <c r="H12" s="44"/>
-      <c r="I12" s="44"/>
-      <c r="J12" s="44"/>
-      <c r="K12" s="44"/>
+      <c r="E12" s="50"/>
+      <c r="F12" s="43"/>
+      <c r="G12" s="43"/>
+      <c r="H12" s="43"/>
+      <c r="I12" s="43"/>
+      <c r="J12" s="43"/>
+      <c r="K12" s="43"/>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B13" s="44" t="s">
+      <c r="B13" s="43" t="s">
         <v>75</v>
       </c>
-      <c r="C13" s="44" t="s">
+      <c r="C13" s="43" t="s">
         <v>76</v>
       </c>
-      <c r="D13" s="53">
+      <c r="D13" s="51">
         <f>+H6+H8</f>
         <v>6.6799999999999998E-2</v>
       </c>
-      <c r="E13" s="44"/>
-      <c r="F13" s="44"/>
-      <c r="G13" s="44"/>
-      <c r="H13" s="44"/>
-      <c r="I13" s="44"/>
-      <c r="J13" s="44"/>
-      <c r="K13" s="44"/>
+      <c r="E13" s="43"/>
+      <c r="F13" s="43"/>
+      <c r="G13" s="43"/>
+      <c r="H13" s="43"/>
+      <c r="I13" s="43"/>
+      <c r="J13" s="43"/>
+      <c r="K13" s="43"/>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B14" s="44" t="s">
+      <c r="B14" s="43" t="s">
         <v>77</v>
       </c>
-      <c r="C14" s="44"/>
-      <c r="D14" s="54">
+      <c r="C14" s="43"/>
+      <c r="D14" s="52">
         <f>+D6*(1+(1-D5)*D7)</f>
         <v>1</v>
       </c>
-      <c r="E14" s="44"/>
-      <c r="F14" s="44"/>
-      <c r="G14" s="44"/>
-      <c r="H14" s="44"/>
-      <c r="I14" s="44"/>
-      <c r="J14" s="44"/>
-      <c r="K14" s="44"/>
+      <c r="E14" s="43"/>
+      <c r="F14" s="43"/>
+      <c r="G14" s="43"/>
+      <c r="H14" s="43"/>
+      <c r="I14" s="43"/>
+      <c r="J14" s="43"/>
+      <c r="K14" s="43"/>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B15" s="44" t="s">
+      <c r="B15" s="43" t="s">
         <v>78</v>
       </c>
-      <c r="C15" s="44"/>
-      <c r="D15" s="53">
+      <c r="C15" s="43"/>
+      <c r="D15" s="51">
         <f>+D14*H5+H6+H7</f>
         <v>0.1416</v>
       </c>
-      <c r="E15" s="44"/>
-      <c r="F15" s="44"/>
-      <c r="G15" s="44"/>
-      <c r="H15" s="44"/>
-      <c r="I15" s="44"/>
-      <c r="J15" s="44"/>
-      <c r="K15" s="44"/>
+      <c r="E15" s="43"/>
+      <c r="F15" s="43"/>
+      <c r="G15" s="43"/>
+      <c r="H15" s="43"/>
+      <c r="I15" s="43"/>
+      <c r="J15" s="43"/>
+      <c r="K15" s="43"/>
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B16" s="44" t="s">
+      <c r="B16" s="43" t="s">
         <v>79</v>
       </c>
-      <c r="C16" s="44" t="s">
+      <c r="C16" s="43" t="s">
         <v>80</v>
       </c>
-      <c r="D16" s="54">
+      <c r="D16" s="52">
         <f>1/(1+D7)</f>
         <v>1</v>
       </c>
-      <c r="E16" s="44"/>
-      <c r="F16" s="44"/>
-      <c r="G16" s="44"/>
-      <c r="H16" s="44"/>
-      <c r="I16" s="44"/>
-      <c r="J16" s="44"/>
-      <c r="K16" s="44"/>
+      <c r="E16" s="43"/>
+      <c r="F16" s="43"/>
+      <c r="G16" s="43"/>
+      <c r="H16" s="43"/>
+      <c r="I16" s="43"/>
+      <c r="J16" s="43"/>
+      <c r="K16" s="43"/>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B17" s="44" t="s">
+      <c r="B17" s="43" t="s">
         <v>81</v>
       </c>
-      <c r="C17" s="44"/>
-      <c r="D17" s="54">
+      <c r="C17" s="43"/>
+      <c r="D17" s="52">
         <f>1-D16</f>
         <v>0</v>
       </c>
-      <c r="E17" s="44"/>
-      <c r="F17" s="44"/>
-      <c r="G17" s="44"/>
-      <c r="H17" s="44"/>
-      <c r="I17" s="44"/>
-      <c r="J17" s="44"/>
-      <c r="K17" s="44"/>
+      <c r="E17" s="43"/>
+      <c r="F17" s="43"/>
+      <c r="G17" s="43"/>
+      <c r="H17" s="43"/>
+      <c r="I17" s="43"/>
+      <c r="J17" s="43"/>
+      <c r="K17" s="43"/>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B18" s="44" t="s">
+      <c r="B18" s="43" t="s">
         <v>72</v>
       </c>
-      <c r="C18" s="44"/>
-      <c r="D18" s="55">
+      <c r="C18" s="43"/>
+      <c r="D18" s="53">
         <f>+D15*D16+D13*(1-D5)*D17</f>
         <v>0.1416</v>
       </c>
-      <c r="E18" s="44"/>
-      <c r="F18" s="44"/>
-      <c r="G18" s="44"/>
-      <c r="H18" s="44"/>
-      <c r="I18" s="44"/>
-      <c r="J18" s="44"/>
-      <c r="K18" s="44"/>
+      <c r="E18" s="43"/>
+      <c r="F18" s="43"/>
+      <c r="G18" s="43"/>
+      <c r="H18" s="43"/>
+      <c r="I18" s="43"/>
+      <c r="J18" s="43"/>
+      <c r="K18" s="43"/>
     </row>
     <row r="24" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B24" s="49" t="s">
+      <c r="B24" s="48" t="s">
         <v>47</v>
       </c>
-      <c r="C24" s="49">
+      <c r="C24" s="48">
         <v>2021</v>
       </c>
-      <c r="D24" s="49" t="s">
+      <c r="D24" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="E24" s="49" t="s">
+      <c r="E24" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="F24" s="49" t="s">
+      <c r="F24" s="48" t="s">
         <v>18</v>
       </c>
-      <c r="G24" s="49" t="s">
+      <c r="G24" s="48" t="s">
         <v>19</v>
       </c>
-      <c r="H24" s="49" t="s">
+      <c r="H24" s="48" t="s">
         <v>20</v>
       </c>
-      <c r="I24" s="49" t="s">
+      <c r="I24" s="48" t="s">
         <v>21</v>
       </c>
-      <c r="J24" s="49" t="s">
+      <c r="J24" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="K24" s="49" t="s">
+      <c r="K24" s="48" t="s">
         <v>23</v>
       </c>
-      <c r="L24" s="39" t="s">
+      <c r="L24" s="38" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="25" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B25" s="40"/>
-      <c r="D25" s="40"/>
-      <c r="E25" s="40"/>
-      <c r="F25" s="41"/>
-      <c r="G25" s="41"/>
-      <c r="H25" s="41"/>
-      <c r="I25" s="41"/>
-      <c r="J25" s="41"/>
-      <c r="K25" s="41"/>
-      <c r="L25" s="41"/>
+      <c r="B25" s="39"/>
+      <c r="D25" s="39"/>
+      <c r="E25" s="39"/>
+      <c r="F25" s="40"/>
+      <c r="G25" s="40"/>
+      <c r="H25" s="40"/>
+      <c r="I25" s="40"/>
+      <c r="J25" s="40"/>
+      <c r="K25" s="40"/>
+      <c r="L25" s="40"/>
     </row>
     <row r="26" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B26" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="D26" s="45">
+      <c r="D26" s="44">
         <f>+IS!C10</f>
         <v>58925344</v>
       </c>
-      <c r="E26" s="45">
+      <c r="E26" s="44">
         <f>+IS!D10</f>
         <v>-5263551</v>
       </c>
-      <c r="F26" s="45">
+      <c r="F26" s="44">
         <f>+IS!E10</f>
         <v>44704805.010372117</v>
       </c>
-      <c r="G26" s="45">
+      <c r="G26" s="44">
         <f>+IS!F10</f>
         <v>193867413.18327528</v>
       </c>
-      <c r="H26" s="45">
+      <c r="H26" s="44">
         <f>+IS!G10</f>
         <v>233150665.85025933</v>
       </c>
-      <c r="I26" s="45">
+      <c r="I26" s="44">
         <f>+IS!H10</f>
         <v>247093692.04232895</v>
       </c>
-      <c r="J26" s="45">
+      <c r="J26" s="44">
         <f>+IS!I10</f>
         <v>277971275.81750989</v>
       </c>
-      <c r="K26" s="45">
+      <c r="K26" s="44">
         <f>+IS!J10</f>
         <v>303471548.11552042</v>
       </c>
-      <c r="L26" s="45"/>
+      <c r="L26" s="44"/>
     </row>
     <row r="27" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B27" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="D27" s="44"/>
-      <c r="E27" s="44"/>
-      <c r="F27" s="45">
+      <c r="D27" s="43"/>
+      <c r="E27" s="43"/>
+      <c r="F27" s="44">
         <f>+F26*$D$5</f>
         <v>15646681.75363024</v>
       </c>
-      <c r="G27" s="45">
+      <c r="G27" s="44">
         <f t="shared" ref="G27:K27" si="0">+G26*$D$5</f>
         <v>67853594.614146352</v>
       </c>
-      <c r="H27" s="45">
+      <c r="H27" s="44">
         <f t="shared" si="0"/>
         <v>81602733.047590762</v>
       </c>
-      <c r="I27" s="45">
+      <c r="I27" s="44">
         <f t="shared" si="0"/>
         <v>86482792.214815125</v>
       </c>
-      <c r="J27" s="45">
+      <c r="J27" s="44">
         <f t="shared" si="0"/>
         <v>97289946.536128461</v>
       </c>
-      <c r="K27" s="45">
+      <c r="K27" s="44">
         <f t="shared" si="0"/>
         <v>106215041.84043214</v>
       </c>
-      <c r="L27" s="44"/>
+      <c r="L27" s="43"/>
     </row>
     <row r="28" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B28" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="D28" s="44"/>
-      <c r="E28" s="44"/>
-      <c r="F28" s="47">
+      <c r="D28" s="43"/>
+      <c r="E28" s="43"/>
+      <c r="F28" s="46">
         <f>+F26-F27</f>
         <v>29058123.256741878</v>
       </c>
-      <c r="G28" s="47">
+      <c r="G28" s="46">
         <f t="shared" ref="G28:K28" si="1">+G26-G27</f>
         <v>126013818.56912893</v>
       </c>
-      <c r="H28" s="47">
+      <c r="H28" s="46">
         <f t="shared" si="1"/>
         <v>151547932.80266857</v>
       </c>
-      <c r="I28" s="47">
+      <c r="I28" s="46">
         <f t="shared" si="1"/>
         <v>160610899.82751381</v>
       </c>
-      <c r="J28" s="47">
+      <c r="J28" s="46">
         <f t="shared" si="1"/>
         <v>180681329.28138143</v>
       </c>
-      <c r="K28" s="47">
+      <c r="K28" s="46">
         <f t="shared" si="1"/>
         <v>197256506.27508828</v>
       </c>
-      <c r="L28" s="47">
+      <c r="L28" s="46">
         <f>+K28*(1+K5)</f>
         <v>203174201.46334094</v>
       </c>
@@ -5575,200 +5577,200 @@
       <c r="B29" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="D29" s="44"/>
-      <c r="E29" s="45">
+      <c r="D29" s="43"/>
+      <c r="E29" s="44">
         <f>+BS!D6-BS!D9</f>
         <v>85537738</v>
       </c>
-      <c r="F29" s="45">
+      <c r="F29" s="44">
         <f>+BS!E6-BS!E9</f>
         <v>91110865.773407996</v>
       </c>
-      <c r="G29" s="45">
+      <c r="G29" s="44">
         <f>+BS!F6-BS!F9</f>
         <v>109298209.89734267</v>
       </c>
-      <c r="H29" s="45">
+      <c r="H29" s="44">
         <f>+BS!G6-BS!G9</f>
         <v>121226255.35605484</v>
       </c>
-      <c r="I29" s="45">
+      <c r="I29" s="44">
         <f>+BS!H6-BS!H9</f>
         <v>133671958.69986923</v>
       </c>
-      <c r="J29" s="45">
+      <c r="J29" s="44">
         <f>+BS!I6-BS!I9</f>
         <v>147395401.18746307</v>
       </c>
-      <c r="K29" s="45">
+      <c r="K29" s="44">
         <f>+BS!J6-BS!J9</f>
         <v>162527762.0117228</v>
       </c>
-      <c r="L29" s="45"/>
+      <c r="L29" s="44"/>
     </row>
     <row r="30" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B30" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="D30" s="44"/>
-      <c r="E30" s="44"/>
-      <c r="F30" s="45">
+      <c r="D30" s="43"/>
+      <c r="E30" s="43"/>
+      <c r="F30" s="44">
         <f t="shared" ref="F30:K30" si="2">+F29-E29</f>
         <v>5573127.7734079957</v>
       </c>
-      <c r="G30" s="45">
+      <c r="G30" s="44">
         <f t="shared" si="2"/>
         <v>18187344.123934671</v>
       </c>
-      <c r="H30" s="45">
+      <c r="H30" s="44">
         <f t="shared" si="2"/>
         <v>11928045.458712175</v>
       </c>
-      <c r="I30" s="45">
+      <c r="I30" s="44">
         <f t="shared" si="2"/>
         <v>12445703.343814388</v>
       </c>
-      <c r="J30" s="45">
+      <c r="J30" s="44">
         <f t="shared" si="2"/>
         <v>13723442.487593845</v>
       </c>
-      <c r="K30" s="45">
+      <c r="K30" s="44">
         <f t="shared" si="2"/>
         <v>15132360.824259728</v>
       </c>
-      <c r="L30" s="45"/>
+      <c r="L30" s="44"/>
     </row>
     <row r="31" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B31" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="D31" s="44"/>
-      <c r="E31" s="44"/>
-      <c r="F31" s="60">
+      <c r="D31" s="43"/>
+      <c r="E31" s="43"/>
+      <c r="F31" s="58">
         <v>0</v>
       </c>
-      <c r="G31" s="60">
+      <c r="G31" s="58">
         <v>0</v>
       </c>
-      <c r="H31" s="60">
+      <c r="H31" s="58">
         <v>0</v>
       </c>
-      <c r="I31" s="60">
+      <c r="I31" s="58">
         <v>0</v>
       </c>
-      <c r="J31" s="60">
+      <c r="J31" s="58">
         <v>0</v>
       </c>
-      <c r="K31" s="60">
+      <c r="K31" s="58">
         <v>0</v>
       </c>
-      <c r="L31" s="45"/>
+      <c r="L31" s="44"/>
     </row>
     <row r="32" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B32" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="D32" s="44"/>
-      <c r="E32" s="44"/>
-      <c r="F32" s="45">
+      <c r="D32" s="43"/>
+      <c r="E32" s="43"/>
+      <c r="F32" s="44">
         <f>+IS!E40</f>
         <v>1556658</v>
       </c>
-      <c r="G32" s="45">
+      <c r="G32" s="44">
         <f>+IS!F40</f>
         <v>1556658</v>
       </c>
-      <c r="H32" s="45">
+      <c r="H32" s="44">
         <f>+IS!G40</f>
         <v>1556658</v>
       </c>
-      <c r="I32" s="45">
+      <c r="I32" s="44">
         <f>+IS!H40</f>
         <v>1556658</v>
       </c>
-      <c r="J32" s="45">
+      <c r="J32" s="44">
         <f>+IS!I40</f>
         <v>1556658</v>
       </c>
-      <c r="K32" s="45">
+      <c r="K32" s="44">
         <f>+IS!J40</f>
         <v>1556658</v>
       </c>
-      <c r="L32" s="45"/>
+      <c r="L32" s="44"/>
     </row>
     <row r="33" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B33" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="D33" s="44"/>
-      <c r="E33" s="44"/>
-      <c r="F33" s="45">
+      <c r="D33" s="43"/>
+      <c r="E33" s="43"/>
+      <c r="F33" s="44">
         <f>+(BS!E5-BS!D5)+IS!E31</f>
         <v>8845303.5857694745</v>
       </c>
-      <c r="G33" s="45">
+      <c r="G33" s="44">
         <f>+(BS!F5-BS!E5)+IS!F31</f>
         <v>25342422.629028976</v>
       </c>
-      <c r="H33" s="45">
+      <c r="H33" s="44">
         <f>+(BS!G5-BS!F5)+IS!G31</f>
         <v>17156389.320413709</v>
       </c>
-      <c r="I33" s="45">
+      <c r="I33" s="44">
         <f>+(BS!H5-BS!G5)+IS!H31</f>
         <v>17833392.434749603</v>
       </c>
-      <c r="J33" s="45">
+      <c r="J33" s="44">
         <f>+(BS!I5-BS!H5)+IS!I31</f>
         <v>19504444.696373582</v>
       </c>
-      <c r="K33" s="45">
+      <c r="K33" s="44">
         <f>+(BS!J5-BS!I5)+IS!J31</f>
         <v>21347055.674045473</v>
       </c>
-      <c r="L33" s="45"/>
+      <c r="L33" s="44"/>
     </row>
     <row r="34" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B34" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="C34" s="61">
+      <c r="C34" s="59">
         <f>-20000000/(1/5*1/3)</f>
         <v>-300000000</v>
       </c>
-      <c r="D34" s="47">
+      <c r="D34" s="46">
         <f t="shared" ref="D34:F34" si="3">+D28-D30+D31+D32-D33</f>
         <v>0</v>
       </c>
-      <c r="E34" s="47">
+      <c r="E34" s="46">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="F34" s="47">
+      <c r="F34" s="46">
         <f t="shared" si="3"/>
         <v>16196349.897564407</v>
       </c>
-      <c r="G34" s="47">
+      <c r="G34" s="46">
         <f>+G28-G30+G31+G32-G33</f>
         <v>84040709.816165283</v>
       </c>
-      <c r="H34" s="47">
+      <c r="H34" s="46">
         <f t="shared" ref="H34:K34" si="4">+H28-H30+H31+H32-H33</f>
         <v>124020156.0235427</v>
       </c>
-      <c r="I34" s="47">
+      <c r="I34" s="46">
         <f t="shared" si="4"/>
         <v>131888462.04894984</v>
       </c>
-      <c r="J34" s="47">
+      <c r="J34" s="46">
         <f t="shared" si="4"/>
         <v>149010100.09741402</v>
       </c>
-      <c r="K34" s="47">
+      <c r="K34" s="46">
         <f t="shared" si="4"/>
         <v>162333747.77678308</v>
       </c>
-      <c r="L34" s="47">
+      <c r="L34" s="46">
         <f>+L28*(1-(K5/K6))/(D18-K5)</f>
         <v>1137848350.4891405</v>
       </c>
@@ -5777,30 +5779,30 @@
       <c r="B35" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="D35" s="44"/>
-      <c r="E35" s="44"/>
-      <c r="F35" s="44"/>
-      <c r="G35" s="48">
+      <c r="D35" s="43"/>
+      <c r="E35" s="43"/>
+      <c r="F35" s="43"/>
+      <c r="G35" s="47">
         <f>1/(1+D18)</f>
         <v>0.87596355991590757</v>
       </c>
-      <c r="H35" s="48">
+      <c r="H35" s="47">
         <f>+G35*$G$35</f>
         <v>0.76731215830054977</v>
       </c>
-      <c r="I35" s="48">
+      <c r="I35" s="47">
         <f>+H35*$G$35</f>
         <v>0.67213748975170795</v>
       </c>
-      <c r="J35" s="48">
+      <c r="J35" s="47">
         <f>+I35*$G$35</f>
         <v>0.58876794827584789</v>
       </c>
-      <c r="K35" s="48">
+      <c r="K35" s="47">
         <f>+J35*$G$35</f>
         <v>0.5157392679360967</v>
       </c>
-      <c r="L35" s="48">
+      <c r="L35" s="47">
         <f>+K35</f>
         <v>0.5157392679360967</v>
       </c>
@@ -5809,200 +5811,197 @@
       <c r="B36" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="D36" s="46"/>
-      <c r="E36" s="46"/>
-      <c r="F36" s="46"/>
-      <c r="G36" s="47">
+      <c r="D36" s="45"/>
+      <c r="E36" s="45"/>
+      <c r="F36" s="45"/>
+      <c r="G36" s="46">
         <f t="shared" ref="G36:L36" si="5">+G35*G34</f>
         <v>73616599.348427907</v>
       </c>
-      <c r="H36" s="47">
+      <c r="H36" s="46">
         <f t="shared" si="5"/>
         <v>95162173.591195479</v>
       </c>
-      <c r="I36" s="47">
+      <c r="I36" s="46">
         <f t="shared" si="5"/>
         <v>88647179.808794543</v>
       </c>
-      <c r="J36" s="47">
+      <c r="J36" s="46">
         <f t="shared" si="5"/>
         <v>87732370.90673317</v>
       </c>
-      <c r="K36" s="47">
+      <c r="K36" s="46">
         <f t="shared" si="5"/>
         <v>83721888.239721075</v>
       </c>
-      <c r="L36" s="47">
+      <c r="L36" s="46">
         <f t="shared" si="5"/>
         <v>586833075.30356455</v>
       </c>
     </row>
     <row r="38" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B38" s="63" t="s">
+      <c r="B38" s="61" t="s">
         <v>91</v>
       </c>
-      <c r="C38" s="64">
+      <c r="C38" s="62">
         <v>4400</v>
       </c>
-      <c r="D38" s="65" t="s">
+      <c r="D38" s="63" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="39" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B39" s="66" t="s">
+      <c r="B39" s="64" t="s">
         <v>93</v>
       </c>
-      <c r="C39" s="67">
+      <c r="C39" s="46">
         <f>+SUM(G36:L36)</f>
         <v>1015713287.1984367</v>
       </c>
-      <c r="D39" s="68">
+      <c r="D39" s="65">
         <f>+C39/$C$38</f>
         <v>230843.92890873563</v>
       </c>
     </row>
     <row r="40" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B40" s="66" t="s">
+      <c r="B40" s="64" t="s">
         <v>48</v>
       </c>
-      <c r="C40" s="69">
+      <c r="C40" s="44">
         <v>0</v>
       </c>
-      <c r="D40" s="70">
+      <c r="D40" s="66">
         <v>0</v>
       </c>
     </row>
     <row r="41" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B41" s="66" t="s">
+      <c r="B41" s="64" t="s">
         <v>83</v>
       </c>
-      <c r="C41" s="69">
+      <c r="C41" s="44">
         <v>0</v>
       </c>
-      <c r="D41" s="70">
+      <c r="D41" s="66">
         <v>0</v>
       </c>
     </row>
     <row r="42" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B42" s="71" t="s">
+      <c r="B42" s="67" t="s">
         <v>84</v>
       </c>
-      <c r="C42" s="67">
+      <c r="C42" s="46">
         <f>+C39+C40+C41</f>
         <v>1015713287.1984367</v>
       </c>
-      <c r="D42" s="68">
+      <c r="D42" s="65">
         <f>+D39+D40+D41</f>
         <v>230843.92890873563</v>
       </c>
     </row>
     <row r="43" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B43" s="72"/>
-      <c r="C43" s="73"/>
-      <c r="D43" s="70"/>
+      <c r="B43" s="68"/>
+      <c r="D43" s="66"/>
     </row>
     <row r="44" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B44" s="72" t="s">
+      <c r="B44" s="68" t="s">
         <v>86</v>
       </c>
-      <c r="C44" s="74">
+      <c r="C44" s="69">
         <v>7</v>
       </c>
-      <c r="D44" s="75">
+      <c r="D44" s="70">
         <f>+C44</f>
         <v>7</v>
       </c>
     </row>
     <row r="45" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B45" s="72" t="s">
+      <c r="B45" s="68" t="s">
         <v>87</v>
       </c>
-      <c r="C45" s="76">
+      <c r="C45" s="10">
         <f>+IS!F42</f>
         <v>285639471.2418111</v>
       </c>
-      <c r="D45" s="77">
+      <c r="D45" s="71">
         <f>+C45/C38</f>
         <v>64918.061645866161</v>
       </c>
     </row>
     <row r="46" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B46" s="78" t="s">
+      <c r="B46" s="72" t="s">
         <v>82</v>
       </c>
-      <c r="C46" s="67">
+      <c r="C46" s="46">
         <f>+C45*C44</f>
         <v>1999476298.6926777</v>
       </c>
-      <c r="D46" s="68">
+      <c r="D46" s="65">
         <f>+C46/C38</f>
         <v>454426.43152106315</v>
       </c>
     </row>
     <row r="47" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B47" s="72"/>
-      <c r="C47" s="73"/>
-      <c r="D47" s="70"/>
+      <c r="B47" s="68"/>
+      <c r="D47" s="66"/>
     </row>
     <row r="48" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B48" s="72" t="s">
+      <c r="B48" s="68" t="s">
         <v>92</v>
       </c>
-      <c r="C48" s="79">
+      <c r="C48" s="73">
         <f>+C34</f>
         <v>-300000000</v>
       </c>
-      <c r="D48" s="80">
+      <c r="D48" s="74">
         <f>+C48/$C$38</f>
         <v>-68181.818181818177</v>
       </c>
-      <c r="E48" s="62">
+      <c r="E48" s="60">
         <v>44561</v>
       </c>
     </row>
     <row r="49" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B49" s="72" t="s">
+      <c r="B49" s="68" t="s">
         <v>82</v>
       </c>
-      <c r="C49" s="76">
+      <c r="C49" s="10">
         <f>+C46</f>
         <v>1999476298.6926777</v>
       </c>
-      <c r="D49" s="77">
+      <c r="D49" s="71">
         <f>+C49/$C$38</f>
         <v>454426.43152106315</v>
       </c>
-      <c r="E49" s="62">
+      <c r="E49" s="60">
         <v>47483</v>
       </c>
     </row>
     <row r="50" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B50" s="72"/>
-      <c r="C50" s="73"/>
-      <c r="D50" s="70"/>
+      <c r="B50" s="68"/>
+      <c r="D50" s="66"/>
     </row>
     <row r="51" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B51" s="78" t="s">
+      <c r="B51" s="72" t="s">
         <v>88</v>
       </c>
-      <c r="C51" s="81">
+      <c r="C51" s="75">
         <f>+IRR(C34:L34)</f>
         <v>0.26614973525058172</v>
       </c>
-      <c r="D51" s="82">
+      <c r="D51" s="76">
         <f>+C51</f>
         <v>0.26614973525058172</v>
       </c>
     </row>
     <row r="52" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B52" s="83" t="s">
+      <c r="B52" s="77" t="s">
         <v>89</v>
       </c>
-      <c r="C52" s="84">
+      <c r="C52" s="78">
         <f>+XIRR(C48:C49,E48:E49)</f>
         <v>0.26737137436866765</v>
       </c>
-      <c r="D52" s="85">
+      <c r="D52" s="79">
         <f>+C52</f>
         <v>0.26737137436866765</v>
       </c>
@@ -6036,213 +6035,213 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:17" ht="18" x14ac:dyDescent="0.35">
-      <c r="B1" s="43" t="s">
+      <c r="B1" s="42" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="4" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B4" s="49" t="s">
+      <c r="B4" s="48" t="s">
         <v>47</v>
       </c>
-      <c r="C4" s="49" t="s">
+      <c r="C4" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="49" t="s">
+      <c r="D4" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="49" t="s">
+      <c r="E4" s="48" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="49" t="s">
+      <c r="F4" s="48" t="s">
         <v>19</v>
       </c>
-      <c r="G4" s="49" t="s">
+      <c r="G4" s="48" t="s">
         <v>20</v>
       </c>
-      <c r="H4" s="49" t="s">
+      <c r="H4" s="48" t="s">
         <v>21</v>
       </c>
-      <c r="I4" s="49" t="s">
+      <c r="I4" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="J4" s="49" t="s">
+      <c r="J4" s="48" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="5" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B5" s="24" t="s">
+      <c r="B5" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="C5" s="38">
+      <c r="C5" s="37">
         <v>72076487</v>
       </c>
-      <c r="D5" s="25">
+      <c r="D5" s="24">
         <f>+C8</f>
         <v>72076487</v>
       </c>
-      <c r="E5" s="30">
+      <c r="E5" s="29">
         <f>D8</f>
         <v>90576197</v>
       </c>
-      <c r="F5" s="30">
+      <c r="F5" s="29">
         <f>E8</f>
         <v>123149659.06905799</v>
       </c>
-      <c r="G5" s="27">
+      <c r="G5" s="26">
         <f>F8</f>
         <v>136401037.76547217</v>
       </c>
-      <c r="H5" s="27">
+      <c r="H5" s="26">
         <f t="shared" ref="H5:J5" si="0">G8</f>
         <v>148712863.92128876</v>
       </c>
-      <c r="I5" s="27">
+      <c r="I5" s="26">
         <f t="shared" si="0"/>
         <v>152209826.53510684</v>
       </c>
-      <c r="J5" s="27">
+      <c r="J5" s="26">
         <f t="shared" si="0"/>
         <v>150202828.54709762</v>
       </c>
-      <c r="K5" s="26"/>
-      <c r="L5" s="26"/>
-      <c r="M5" s="26"/>
-      <c r="N5" s="26"/>
-      <c r="O5" s="26"/>
-      <c r="P5" s="26"/>
-      <c r="Q5" s="26"/>
+      <c r="K5" s="25"/>
+      <c r="L5" s="25"/>
+      <c r="M5" s="25"/>
+      <c r="N5" s="25"/>
+      <c r="O5" s="25"/>
+      <c r="P5" s="25"/>
+      <c r="Q5" s="25"/>
     </row>
     <row r="6" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B6" s="24" t="s">
+      <c r="B6" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="C6" s="26">
+      <c r="C6" s="25">
         <f>C8-C5-C7</f>
         <v>33568463</v>
       </c>
-      <c r="D6" s="26">
+      <c r="D6" s="25">
         <f>D8-D5-D7</f>
         <v>98040502</v>
       </c>
-      <c r="E6" s="35">
+      <c r="E6" s="34">
         <f>+D6*(1+E9)</f>
         <v>101471919.56999999</v>
       </c>
-      <c r="F6" s="27">
+      <c r="F6" s="26">
         <f t="shared" ref="F6:J6" si="1">+E6*(1+F9)</f>
         <v>105023436.75494999</v>
       </c>
-      <c r="G6" s="27">
+      <c r="G6" s="26">
         <f t="shared" si="1"/>
         <v>108699257.04137322</v>
       </c>
-      <c r="H6" s="27">
+      <c r="H6" s="26">
         <f t="shared" si="1"/>
         <v>112503731.03782128</v>
       </c>
-      <c r="I6" s="27">
+      <c r="I6" s="26">
         <f t="shared" si="1"/>
         <v>116441361.62414502</v>
       </c>
-      <c r="J6" s="27">
+      <c r="J6" s="26">
         <f t="shared" si="1"/>
         <v>120516809.28099008</v>
       </c>
-      <c r="K6" s="26"/>
-      <c r="L6" s="26"/>
-      <c r="M6" s="26"/>
-      <c r="N6" s="26"/>
-      <c r="O6" s="26"/>
-      <c r="P6" s="26"/>
-      <c r="Q6" s="26"/>
+      <c r="K6" s="25"/>
+      <c r="L6" s="25"/>
+      <c r="M6" s="25"/>
+      <c r="N6" s="25"/>
+      <c r="O6" s="25"/>
+      <c r="P6" s="25"/>
+      <c r="Q6" s="25"/>
     </row>
     <row r="7" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B7" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="C7" s="36">
+      <c r="C7" s="35">
         <f>-IS!C33</f>
         <v>-33568463</v>
       </c>
-      <c r="D7" s="36">
+      <c r="D7" s="35">
         <f>-IS!D33</f>
         <v>-79540792</v>
       </c>
-      <c r="E7" s="31">
+      <c r="E7" s="30">
         <f>-IS!E33</f>
         <v>-68898457.500942007</v>
       </c>
-      <c r="F7" s="31">
+      <c r="F7" s="30">
         <f>-IS!F33</f>
         <v>-91772058.058535814</v>
       </c>
-      <c r="G7" s="31">
+      <c r="G7" s="30">
         <f>-IS!G33</f>
         <v>-96387430.885556638</v>
       </c>
-      <c r="H7" s="31">
+      <c r="H7" s="30">
         <f>-IS!H33</f>
         <v>-109006768.42400318</v>
       </c>
-      <c r="I7" s="31">
+      <c r="I7" s="30">
         <f>-IS!I33</f>
         <v>-118448359.61215426</v>
       </c>
-      <c r="J7" s="31">
+      <c r="J7" s="30">
         <f>-IS!J33</f>
         <v>-131325554.80965064</v>
       </c>
-      <c r="K7" s="33"/>
-      <c r="L7" s="33"/>
-      <c r="M7" s="33"/>
-      <c r="N7" s="33"/>
-      <c r="O7" s="33"/>
-      <c r="P7" s="33"/>
-      <c r="Q7" s="33"/>
+      <c r="K7" s="32"/>
+      <c r="L7" s="32"/>
+      <c r="M7" s="32"/>
+      <c r="N7" s="32"/>
+      <c r="O7" s="32"/>
+      <c r="P7" s="32"/>
+      <c r="Q7" s="32"/>
     </row>
     <row r="8" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="28" t="s">
+      <c r="B8" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="C8" s="37">
+      <c r="C8" s="36">
         <f>+BS!C6</f>
         <v>72076487</v>
       </c>
-      <c r="D8" s="37">
+      <c r="D8" s="36">
         <f>+BS!D6</f>
         <v>90576197</v>
       </c>
-      <c r="E8" s="32">
+      <c r="E8" s="31">
         <f>+SUM(E5:E7)</f>
         <v>123149659.06905799</v>
       </c>
-      <c r="F8" s="32">
+      <c r="F8" s="31">
         <f t="shared" ref="F8:J8" si="2">+SUM(F5:F7)</f>
         <v>136401037.76547217</v>
       </c>
-      <c r="G8" s="32">
+      <c r="G8" s="31">
         <f t="shared" si="2"/>
         <v>148712863.92128876</v>
       </c>
-      <c r="H8" s="32">
+      <c r="H8" s="31">
         <f t="shared" si="2"/>
         <v>152209826.53510684</v>
       </c>
-      <c r="I8" s="32">
+      <c r="I8" s="31">
         <f t="shared" si="2"/>
         <v>150202828.54709762</v>
       </c>
-      <c r="J8" s="32">
+      <c r="J8" s="31">
         <f t="shared" si="2"/>
         <v>139394083.01843703</v>
       </c>
-      <c r="K8" s="29"/>
-      <c r="L8" s="29"/>
-      <c r="M8" s="29"/>
-      <c r="N8" s="29"/>
-      <c r="O8" s="29"/>
-      <c r="P8" s="29"/>
-      <c r="Q8" s="29"/>
+      <c r="K8" s="28"/>
+      <c r="L8" s="28"/>
+      <c r="M8" s="28"/>
+      <c r="N8" s="28"/>
+      <c r="O8" s="28"/>
+      <c r="P8" s="28"/>
+      <c r="Q8" s="28"/>
     </row>
     <row r="9" spans="2:17" x14ac:dyDescent="0.3">
       <c r="E9" s="16">

</xml_diff>